<commit_message>
Corrected mistake in raw 2020 results
</commit_message>
<xml_diff>
--- a/data/raw_election_results_1st_round/munic2020-paris-ardmnt.xlsx
+++ b/data/raw_election_results_1st_round/munic2020-paris-ardmnt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex_andorra/repos/pollsposition_models/data/raw_election_results_1st_round/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8578109C-9E63-A64E-8795-61CF2E7916A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BFEC41-10BD-FA4E-92D8-C899EE651468}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="600" windowWidth="31860" windowHeight="18280" xr2:uid="{93B5F9A3-1B7F-A84B-AB26-FCB4479152F4}"/>
   </bookViews>
@@ -1869,8 +1869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F15EA1B7-D331-9B4E-A11E-474226A4DA48}">
   <dimension ref="A1:GD18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="GG8" sqref="GG8"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="L17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9317,7 +9317,7 @@
         <v>1</v>
       </c>
       <c r="T17" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="U17" t="s">
         <v>47</v>

</xml_diff>